<commit_message>
Gave board of management a name and marked items in the vision statement that should be refined
</commit_message>
<xml_diff>
--- a/docs/visionstatement.xlsx
+++ b/docs/visionstatement.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>For:</t>
   </si>
@@ -48,12 +48,15 @@
     <t>Wish for optimal and maximal utilization of their lanes, thus yielding larger 
 profits</t>
   </si>
+  <si>
+    <t>Revamp this</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,13 +64,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -79,16 +94,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -388,19 +406,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +427,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -416,15 +435,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -432,12 +454,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>